<commit_message>
completed selenium with java
</commit_message>
<xml_diff>
--- a/TestData/Book2.xlsx
+++ b/TestData/Book2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\java practice\Java_41\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCDA9D5E-2C78-4A39-B61C-9C3AF04C0F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8238C418-5C62-4AF8-8EF2-4C9B52DCF4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8987F4FF-F22D-4AD2-8E19-FC4284154FFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{8987F4FF-F22D-4AD2-8E19-FC4284154FFA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login1" sheetId="1" r:id="rId1"/>
+    <sheet name="GTM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,19 +37,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>heoifoew</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>id_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first name </t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>aadhaar</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>Shekhar</t>
+  </si>
+  <si>
+    <t>Palo</t>
+  </si>
+  <si>
+    <t>shekhar123@test.com</t>
+  </si>
+  <si>
+    <t>CHUPK3570Q</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +119,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,20 +461,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58B3C62-E39B-4CC6-B398-E4ADED0929EB}">
-  <dimension ref="D1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9F3EF4-B767-452E-8F44-EDEA176161AC}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>8896147850</v>
+      </c>
+      <c r="E2">
+        <v>987286540931</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CDD84886-391D-4406-A1B8-DD178112EB59}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>